<commit_message>
check if file changed support
</commit_message>
<xml_diff>
--- a/public/excel/database.xlsx
+++ b/public/excel/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PProject\dbs-shiorim\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0B04D8-6729-4EA9-962A-F1FD8975CC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24282F29-DAAC-416D-831F-0FF5069DCC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="874" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,28 @@
     <sheet name="News" sheetId="55" r:id="rId4"/>
     <sheet name="Birthday" sheetId="56" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="210">
   <si>
     <t>End</t>
   </si>
@@ -641,6 +652,24 @@
   </si>
   <si>
     <t>רן</t>
+  </si>
+  <si>
+    <t>אומנות מלאכת יד</t>
+  </si>
+  <si>
+    <t>אנגלית</t>
+  </si>
+  <si>
+    <t>יוגה</t>
+  </si>
+  <si>
+    <t>מדעים</t>
+  </si>
+  <si>
+    <t>נגרות</t>
+  </si>
+  <si>
+    <t>תרפיה במוזיקה</t>
   </si>
 </sst>
 </file>
@@ -698,7 +727,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -708,28 +737,17 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -739,7 +757,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -765,10 +783,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1248,6 +1267,7 @@
       <c r="B8" s="3">
         <v>0.39583333333333331</v>
       </c>
+      <c r="D8" s="10"/>
       <c r="G8" s="9"/>
       <c r="H8" t="s">
         <v>20</v>
@@ -1761,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E363FBF9-84D0-4B20-87A9-83BB83FDD08A}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView rightToLeft="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1770,20 +1790,20 @@
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="10" customFormat="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="10" customFormat="1">
+      <c r="A2" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="10" t="s">
-        <v>94</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>54</v>
@@ -1791,15 +1811,10 @@
       <c r="C2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>54</v>
@@ -1813,31 +1828,36 @@
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="1:17" s="10" customFormat="1">
+    <row r="4" spans="1:17">
       <c r="A4" s="10" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>65</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:17" s="10" customFormat="1">
       <c r="A5" s="10" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="10" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>124</v>
@@ -1848,7 +1868,7 @@
     </row>
     <row r="7" spans="1:17" s="10" customFormat="1">
       <c r="A7" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>124</v>
@@ -1859,10 +1879,10 @@
     </row>
     <row r="8" spans="1:17" s="10" customFormat="1">
       <c r="A8" s="10" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>56</v>
@@ -1870,7 +1890,7 @@
     </row>
     <row r="9" spans="1:17" s="10" customFormat="1">
       <c r="A9" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>57</v>
@@ -1881,7 +1901,7 @@
     </row>
     <row r="10" spans="1:17" s="10" customFormat="1">
       <c r="A10" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>57</v>
@@ -1892,18 +1912,18 @@
     </row>
     <row r="11" spans="1:17" s="10" customFormat="1">
       <c r="A11" s="10" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="10" customFormat="1">
       <c r="A12" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>53</v>
@@ -1912,47 +1932,41 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" t="s">
-        <v>123</v>
-      </c>
-      <c r="M13" s="10"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="2"/>
+    <row r="13" spans="1:17" s="10" customFormat="1">
+      <c r="A13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="L14" s="10"/>
+        <v>123</v>
+      </c>
       <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
       <c r="O14" s="9"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="10" t="s">
-        <v>78</v>
+      <c r="A15" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -1962,13 +1976,13 @@
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" t="s">
         <v>123</v>
       </c>
       <c r="L16" s="10"/>
@@ -1979,14 +1993,14 @@
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
+      <c r="A17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -1997,24 +2011,24 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>46</v>
@@ -2025,35 +2039,35 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
+        <v>12</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" t="s">
-        <v>9</v>
+      <c r="A21" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -2063,11 +2077,11 @@
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>48</v>
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>45</v>
@@ -2081,9 +2095,9 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -2093,14 +2107,15 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>46</v>
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>45</v>
@@ -2109,51 +2124,50 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
+        <v>16</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" t="s">
         <v>59</v>
       </c>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" t="s">
-        <v>129</v>
+        <v>97</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
@@ -2163,14 +2177,14 @@
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" t="s">
-        <v>23</v>
+      <c r="A28" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
@@ -2181,13 +2195,13 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
@@ -2197,14 +2211,14 @@
       <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="10" t="s">
-        <v>22</v>
+      <c r="A30" t="s">
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
@@ -2215,44 +2229,45 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="10" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
-      <c r="P31" s="9"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
       <c r="Q31" s="2"/>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
-      <c r="O32" s="9"/>
+      <c r="N32" s="10"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="10" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" t="s">
         <v>51</v>
       </c>
       <c r="L33" s="10"/>
@@ -2262,42 +2277,41 @@
       <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" t="s">
-        <v>39</v>
+      <c r="A34" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>51</v>
       </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="2"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="10" t="s">
-        <v>79</v>
+      <c r="A35" t="s">
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>123</v>
+        <v>54</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
       <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="2" t="s">
-        <v>36</v>
+      <c r="A36" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="B36" t="s">
         <v>66</v>
@@ -2306,135 +2320,141 @@
         <v>123</v>
       </c>
       <c r="L36" s="10"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
       <c r="Q36" s="2"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="10" t="s">
-        <v>44</v>
+      <c r="A37" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="L37" s="10"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
-      <c r="Q37" s="10"/>
-    </row>
-    <row r="38" spans="1:17" s="10" customFormat="1">
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>132</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="10"/>
+    </row>
+    <row r="39" spans="1:17" s="10" customFormat="1">
+      <c r="A39" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="10"/>
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" t="s">
         <v>63</v>
       </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="10"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="10" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
-      <c r="A43" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="B43" t="s">
         <v>66</v>
       </c>
       <c r="C43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="A44" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>48</v>
@@ -2445,7 +2465,7 @@
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>48</v>
@@ -2456,29 +2476,29 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" t="s">
-        <v>50</v>
+        <v>17</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>47</v>
@@ -2489,21 +2509,21 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B52" t="s">
-        <v>133</v>
-      </c>
-      <c r="C52" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
         <v>24</v>
@@ -2511,24 +2531,24 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B55" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C55" s="10" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2576,8 +2596,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C59">
-    <sortCondition ref="A22:A59"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C59">
+    <sortCondition ref="A23:A59"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2587,15 +2607,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AFCDCB-BA3E-441A-848B-9F8AB33FF68E}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:AH80"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:34">
       <c r="A1" s="12" t="s">
         <v>134</v>
       </c>
@@ -2605,9 +2638,101 @@
       <c r="C1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" s="12" t="s">
         <v>137</v>
       </c>
@@ -2617,8 +2742,39 @@
       <c r="C2" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" s="12" t="s">
         <v>138</v>
       </c>
@@ -2628,8 +2784,39 @@
       <c r="C3" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" s="12" t="s">
         <v>139</v>
       </c>
@@ -2639,8 +2826,39 @@
       <c r="C4" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" s="12" t="s">
         <v>140</v>
       </c>
@@ -2650,8 +2868,39 @@
       <c r="C5" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" s="12" t="s">
         <v>141</v>
       </c>
@@ -2661,8 +2910,39 @@
       <c r="C6" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7" s="12" t="s">
         <v>142</v>
       </c>
@@ -2672,8 +2952,39 @@
       <c r="C7" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+    </row>
+    <row r="8" spans="1:34">
       <c r="A8" s="12" t="s">
         <v>143</v>
       </c>
@@ -2683,8 +2994,39 @@
       <c r="C8" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+    </row>
+    <row r="9" spans="1:34">
       <c r="A9" s="12" t="s">
         <v>124</v>
       </c>
@@ -2694,8 +3036,39 @@
       <c r="C9" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+    </row>
+    <row r="10" spans="1:34">
       <c r="A10" s="12" t="s">
         <v>144</v>
       </c>
@@ -2705,8 +3078,39 @@
       <c r="C10" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+    </row>
+    <row r="11" spans="1:34">
       <c r="A11" s="12" t="s">
         <v>145</v>
       </c>
@@ -2716,8 +3120,39 @@
       <c r="C11" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+    </row>
+    <row r="12" spans="1:34">
       <c r="A12" s="12" t="s">
         <v>146</v>
       </c>
@@ -2727,8 +3162,39 @@
       <c r="C12" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+    </row>
+    <row r="13" spans="1:34">
       <c r="A13" s="12" t="s">
         <v>147</v>
       </c>
@@ -2738,8 +3204,39 @@
       <c r="C13" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="13"/>
+    </row>
+    <row r="14" spans="1:34">
       <c r="A14" s="12" t="s">
         <v>148</v>
       </c>
@@ -2749,19 +3246,81 @@
       <c r="C14" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="13"/>
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="13"/>
+      <c r="AH14" s="13"/>
+    </row>
+    <row r="15" spans="1:34">
       <c r="A15" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>7</v>
       </c>
       <c r="C15" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="13"/>
+      <c r="AG15" s="13"/>
+      <c r="AH15" s="13"/>
+    </row>
+    <row r="16" spans="1:34">
       <c r="A16" s="12" t="s">
         <v>150</v>
       </c>
@@ -2771,8 +3330,39 @@
       <c r="C16" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="13"/>
+      <c r="AF16" s="13"/>
+      <c r="AG16" s="13"/>
+      <c r="AH16" s="13"/>
+    </row>
+    <row r="17" spans="1:34">
       <c r="A17" s="12" t="s">
         <v>151</v>
       </c>
@@ -2782,8 +3372,39 @@
       <c r="C17" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+      <c r="AH17" s="13"/>
+    </row>
+    <row r="18" spans="1:34">
       <c r="A18" s="12" t="s">
         <v>152</v>
       </c>
@@ -2793,8 +3414,39 @@
       <c r="C18" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="13"/>
+      <c r="AC18" s="13"/>
+      <c r="AD18" s="13"/>
+      <c r="AE18" s="13"/>
+      <c r="AF18" s="13"/>
+      <c r="AG18" s="13"/>
+      <c r="AH18" s="13"/>
+    </row>
+    <row r="19" spans="1:34">
       <c r="A19" s="12" t="s">
         <v>153</v>
       </c>
@@ -2804,8 +3456,39 @@
       <c r="C19" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+    </row>
+    <row r="20" spans="1:34">
       <c r="A20" s="12" t="s">
         <v>154</v>
       </c>
@@ -2815,8 +3498,39 @@
       <c r="C20" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="13"/>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="13"/>
+      <c r="AF20" s="13"/>
+      <c r="AG20" s="13"/>
+      <c r="AH20" s="13"/>
+    </row>
+    <row r="21" spans="1:34">
       <c r="A21" s="12" t="s">
         <v>155</v>
       </c>
@@ -2826,19 +3540,81 @@
       <c r="C21" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+      <c r="AH21" s="13"/>
+    </row>
+    <row r="22" spans="1:34">
       <c r="A22" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>6</v>
       </c>
       <c r="C22" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="13"/>
+      <c r="AF22" s="13"/>
+      <c r="AG22" s="13"/>
+      <c r="AH22" s="13"/>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23" s="12" t="s">
         <v>157</v>
       </c>
@@ -2848,8 +3624,39 @@
       <c r="C23" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="13"/>
+      <c r="AD23" s="13"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
+      <c r="AH23" s="13"/>
+    </row>
+    <row r="24" spans="1:34">
       <c r="A24" s="12" t="s">
         <v>158</v>
       </c>
@@ -2859,8 +3666,39 @@
       <c r="C24" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
+      <c r="AF24" s="13"/>
+      <c r="AG24" s="13"/>
+      <c r="AH24" s="13"/>
+    </row>
+    <row r="25" spans="1:34">
       <c r="A25" s="12" t="s">
         <v>159</v>
       </c>
@@ -2870,8 +3708,39 @@
       <c r="C25" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="13"/>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="13"/>
+      <c r="AH25" s="13"/>
+    </row>
+    <row r="26" spans="1:34">
       <c r="A26" s="12" t="s">
         <v>62</v>
       </c>
@@ -2881,8 +3750,39 @@
       <c r="C26" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+      <c r="Z26" s="13"/>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="13"/>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="13"/>
+      <c r="AE26" s="13"/>
+      <c r="AF26" s="13"/>
+      <c r="AG26" s="13"/>
+      <c r="AH26" s="13"/>
+    </row>
+    <row r="27" spans="1:34">
       <c r="A27" s="12" t="s">
         <v>160</v>
       </c>
@@ -2892,8 +3792,39 @@
       <c r="C27" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="13"/>
+      <c r="AC27" s="13"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="13"/>
+      <c r="AH27" s="13"/>
+    </row>
+    <row r="28" spans="1:34">
       <c r="A28" s="12" t="s">
         <v>161</v>
       </c>
@@ -2903,8 +3834,39 @@
       <c r="C28" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="13"/>
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="13"/>
+      <c r="AC28" s="13"/>
+      <c r="AD28" s="13"/>
+      <c r="AE28" s="13"/>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="13"/>
+      <c r="AH28" s="13"/>
+    </row>
+    <row r="29" spans="1:34">
       <c r="A29" s="12" t="s">
         <v>162</v>
       </c>
@@ -2914,8 +3876,39 @@
       <c r="C29" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="13"/>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="13"/>
+      <c r="AE29" s="13"/>
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="13"/>
+      <c r="AH29" s="13"/>
+    </row>
+    <row r="30" spans="1:34">
       <c r="A30" s="12" t="s">
         <v>163</v>
       </c>
@@ -2925,8 +3918,39 @@
       <c r="C30" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="13"/>
+      <c r="AC30" s="13"/>
+      <c r="AD30" s="13"/>
+      <c r="AE30" s="13"/>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="13"/>
+      <c r="AH30" s="13"/>
+    </row>
+    <row r="31" spans="1:34">
       <c r="A31" s="12" t="s">
         <v>164</v>
       </c>
@@ -2936,8 +3960,39 @@
       <c r="C31" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="13"/>
+      <c r="AC31" s="13"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="13"/>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="13"/>
+      <c r="AH31" s="13"/>
+    </row>
+    <row r="32" spans="1:34">
       <c r="A32" s="12" t="s">
         <v>165</v>
       </c>
@@ -2947,8 +4002,39 @@
       <c r="C32" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="13"/>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="13"/>
+      <c r="AF32" s="13"/>
+      <c r="AG32" s="13"/>
+      <c r="AH32" s="13"/>
+    </row>
+    <row r="33" spans="1:34">
       <c r="A33" s="12" t="s">
         <v>166</v>
       </c>
@@ -2958,8 +4044,39 @@
       <c r="C33" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="13"/>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="13"/>
+      <c r="AC33" s="13"/>
+      <c r="AD33" s="13"/>
+      <c r="AE33" s="13"/>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="13"/>
+      <c r="AH33" s="13"/>
+    </row>
+    <row r="34" spans="1:34">
       <c r="A34" s="12" t="s">
         <v>167</v>
       </c>
@@ -2969,8 +4086,39 @@
       <c r="C34" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+      <c r="Z34" s="13"/>
+      <c r="AA34" s="13"/>
+      <c r="AB34" s="13"/>
+      <c r="AC34" s="13"/>
+      <c r="AD34" s="13"/>
+      <c r="AE34" s="13"/>
+      <c r="AF34" s="13"/>
+      <c r="AG34" s="13"/>
+      <c r="AH34" s="13"/>
+    </row>
+    <row r="35" spans="1:34">
       <c r="A35" s="12" t="s">
         <v>168</v>
       </c>
@@ -2980,468 +4128,1739 @@
       <c r="C35" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="14" t="s">
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+      <c r="W35" s="13"/>
+      <c r="X35" s="13"/>
+      <c r="Y35" s="13"/>
+      <c r="Z35" s="13"/>
+      <c r="AA35" s="13"/>
+      <c r="AB35" s="13"/>
+      <c r="AC35" s="13"/>
+      <c r="AD35" s="13"/>
+      <c r="AE35" s="13"/>
+      <c r="AF35" s="13"/>
+      <c r="AG35" s="13"/>
+      <c r="AH35" s="13"/>
+    </row>
+    <row r="36" spans="1:34">
+      <c r="A36" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="12">
         <v>5</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="14" t="s">
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
+      <c r="AB36" s="13"/>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="13"/>
+      <c r="AF36" s="13"/>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="13"/>
+    </row>
+    <row r="37" spans="1:34">
+      <c r="A37" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="12">
         <v>5</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="14" t="s">
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="13"/>
+      <c r="AA37" s="13"/>
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="13"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="13"/>
+    </row>
+    <row r="38" spans="1:34">
+      <c r="A38" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="12">
         <v>5</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="14" t="s">
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13"/>
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="13"/>
+      <c r="AF38" s="13"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="13"/>
+    </row>
+    <row r="39" spans="1:34">
+      <c r="A39" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="12">
         <v>4</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="14" t="s">
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="13"/>
+      <c r="Y39" s="13"/>
+      <c r="Z39" s="13"/>
+      <c r="AA39" s="13"/>
+      <c r="AB39" s="13"/>
+      <c r="AC39" s="13"/>
+      <c r="AD39" s="13"/>
+      <c r="AE39" s="13"/>
+      <c r="AF39" s="13"/>
+      <c r="AG39" s="13"/>
+      <c r="AH39" s="13"/>
+    </row>
+    <row r="40" spans="1:34">
+      <c r="A40" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="12">
         <v>4</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="14" t="s">
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+      <c r="W40" s="13"/>
+      <c r="X40" s="13"/>
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="13"/>
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="13"/>
+      <c r="AC40" s="13"/>
+      <c r="AD40" s="13"/>
+      <c r="AE40" s="13"/>
+      <c r="AF40" s="13"/>
+      <c r="AG40" s="13"/>
+      <c r="AH40" s="13"/>
+    </row>
+    <row r="41" spans="1:34">
+      <c r="A41" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>4</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="14" t="s">
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="13"/>
+      <c r="AA41" s="13"/>
+      <c r="AB41" s="13"/>
+      <c r="AC41" s="13"/>
+      <c r="AD41" s="13"/>
+      <c r="AE41" s="13"/>
+      <c r="AF41" s="13"/>
+      <c r="AG41" s="13"/>
+      <c r="AH41" s="13"/>
+    </row>
+    <row r="42" spans="1:34">
+      <c r="A42" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <v>4</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="14" t="s">
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="13"/>
+      <c r="AF42" s="13"/>
+      <c r="AG42" s="13"/>
+      <c r="AH42" s="13"/>
+    </row>
+    <row r="43" spans="1:34">
+      <c r="A43" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="12">
         <v>4</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="14" t="s">
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13"/>
+      <c r="AC43" s="13"/>
+      <c r="AD43" s="13"/>
+      <c r="AE43" s="13"/>
+      <c r="AF43" s="13"/>
+      <c r="AG43" s="13"/>
+      <c r="AH43" s="13"/>
+    </row>
+    <row r="44" spans="1:34">
+      <c r="A44" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="B44" s="14">
+      <c r="B44" s="12">
         <v>4</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="14" t="s">
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+      <c r="W44" s="13"/>
+      <c r="X44" s="13"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="13"/>
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="13"/>
+      <c r="AC44" s="13"/>
+      <c r="AD44" s="13"/>
+      <c r="AE44" s="13"/>
+      <c r="AF44" s="13"/>
+      <c r="AG44" s="13"/>
+      <c r="AH44" s="13"/>
+    </row>
+    <row r="45" spans="1:34">
+      <c r="A45" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45" s="12">
         <v>4</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="14" t="s">
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13"/>
+      <c r="AC45" s="13"/>
+      <c r="AD45" s="13"/>
+      <c r="AE45" s="13"/>
+      <c r="AF45" s="13"/>
+      <c r="AG45" s="13"/>
+      <c r="AH45" s="13"/>
+    </row>
+    <row r="46" spans="1:34">
+      <c r="A46" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="12">
         <v>4</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="14" t="s">
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="13"/>
+      <c r="X46" s="13"/>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="13"/>
+      <c r="AD46" s="13"/>
+      <c r="AE46" s="13"/>
+      <c r="AF46" s="13"/>
+      <c r="AG46" s="13"/>
+      <c r="AH46" s="13"/>
+    </row>
+    <row r="47" spans="1:34">
+      <c r="A47" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="12">
         <v>4</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="14" t="s">
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="13"/>
+      <c r="AC47" s="13"/>
+      <c r="AD47" s="13"/>
+      <c r="AE47" s="13"/>
+      <c r="AF47" s="13"/>
+      <c r="AG47" s="13"/>
+      <c r="AH47" s="13"/>
+    </row>
+    <row r="48" spans="1:34">
+      <c r="A48" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="12">
         <v>4</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="14" t="s">
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="13"/>
+      <c r="X48" s="13"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+      <c r="AC48" s="13"/>
+      <c r="AD48" s="13"/>
+      <c r="AE48" s="13"/>
+      <c r="AF48" s="13"/>
+      <c r="AG48" s="13"/>
+      <c r="AH48" s="13"/>
+    </row>
+    <row r="49" spans="1:34">
+      <c r="A49" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="14">
+      <c r="B49" s="12">
         <v>4</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="14" t="s">
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="13"/>
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="13"/>
+      <c r="AF49" s="13"/>
+      <c r="AG49" s="13"/>
+      <c r="AH49" s="13"/>
+    </row>
+    <row r="50" spans="1:34">
+      <c r="A50" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B50" s="12">
         <v>3</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="14" t="s">
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="13"/>
+      <c r="W50" s="13"/>
+      <c r="X50" s="13"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="13"/>
+      <c r="AC50" s="13"/>
+      <c r="AD50" s="13"/>
+      <c r="AE50" s="13"/>
+      <c r="AF50" s="13"/>
+      <c r="AG50" s="13"/>
+      <c r="AH50" s="13"/>
+    </row>
+    <row r="51" spans="1:34">
+      <c r="A51" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51" s="12">
         <v>3</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="14" t="s">
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="13"/>
+      <c r="X51" s="13"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="13"/>
+      <c r="AA51" s="13"/>
+      <c r="AB51" s="13"/>
+      <c r="AC51" s="13"/>
+      <c r="AD51" s="13"/>
+      <c r="AE51" s="13"/>
+      <c r="AF51" s="13"/>
+      <c r="AG51" s="13"/>
+      <c r="AH51" s="13"/>
+    </row>
+    <row r="52" spans="1:34">
+      <c r="A52" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B52" s="14">
+      <c r="B52" s="12">
         <v>3</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="14" t="s">
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13"/>
+      <c r="V52" s="13"/>
+      <c r="W52" s="13"/>
+      <c r="X52" s="13"/>
+      <c r="Y52" s="13"/>
+      <c r="Z52" s="13"/>
+      <c r="AA52" s="13"/>
+      <c r="AB52" s="13"/>
+      <c r="AC52" s="13"/>
+      <c r="AD52" s="13"/>
+      <c r="AE52" s="13"/>
+      <c r="AF52" s="13"/>
+      <c r="AG52" s="13"/>
+      <c r="AH52" s="13"/>
+    </row>
+    <row r="53" spans="1:34">
+      <c r="A53" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B53" s="14">
+      <c r="B53" s="12">
         <v>3</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="14" t="s">
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="13"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13"/>
+      <c r="V53" s="13"/>
+      <c r="W53" s="13"/>
+      <c r="X53" s="13"/>
+      <c r="Y53" s="13"/>
+      <c r="Z53" s="13"/>
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="13"/>
+      <c r="AC53" s="13"/>
+      <c r="AD53" s="13"/>
+      <c r="AE53" s="13"/>
+      <c r="AF53" s="13"/>
+      <c r="AG53" s="13"/>
+      <c r="AH53" s="13"/>
+    </row>
+    <row r="54" spans="1:34">
+      <c r="A54" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="B54" s="14">
+      <c r="B54" s="12">
         <v>3</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="14" t="s">
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13"/>
+      <c r="S54" s="13"/>
+      <c r="T54" s="13"/>
+      <c r="U54" s="13"/>
+      <c r="V54" s="13"/>
+      <c r="W54" s="13"/>
+      <c r="X54" s="13"/>
+      <c r="Y54" s="13"/>
+      <c r="Z54" s="13"/>
+      <c r="AA54" s="13"/>
+      <c r="AB54" s="13"/>
+      <c r="AC54" s="13"/>
+      <c r="AD54" s="13"/>
+      <c r="AE54" s="13"/>
+      <c r="AF54" s="13"/>
+      <c r="AG54" s="13"/>
+      <c r="AH54" s="13"/>
+    </row>
+    <row r="55" spans="1:34">
+      <c r="A55" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="B55" s="14">
+      <c r="B55" s="12">
         <v>3</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="14" t="s">
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="13"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="13"/>
+      <c r="W55" s="13"/>
+      <c r="X55" s="13"/>
+      <c r="Y55" s="13"/>
+      <c r="Z55" s="13"/>
+      <c r="AA55" s="13"/>
+      <c r="AB55" s="13"/>
+      <c r="AC55" s="13"/>
+      <c r="AD55" s="13"/>
+      <c r="AE55" s="13"/>
+      <c r="AF55" s="13"/>
+      <c r="AG55" s="13"/>
+      <c r="AH55" s="13"/>
+    </row>
+    <row r="56" spans="1:34">
+      <c r="A56" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B56" s="14">
+      <c r="B56" s="12">
         <v>3</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="14" t="s">
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="13"/>
+      <c r="U56" s="13"/>
+      <c r="V56" s="13"/>
+      <c r="W56" s="13"/>
+      <c r="X56" s="13"/>
+      <c r="Y56" s="13"/>
+      <c r="Z56" s="13"/>
+      <c r="AA56" s="13"/>
+      <c r="AB56" s="13"/>
+      <c r="AC56" s="13"/>
+      <c r="AD56" s="13"/>
+      <c r="AE56" s="13"/>
+      <c r="AF56" s="13"/>
+      <c r="AG56" s="13"/>
+      <c r="AH56" s="13"/>
+    </row>
+    <row r="57" spans="1:34">
+      <c r="A57" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B57" s="14">
+      <c r="B57" s="12">
         <v>3</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="14" t="s">
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="13"/>
+      <c r="W57" s="13"/>
+      <c r="X57" s="13"/>
+      <c r="Y57" s="13"/>
+      <c r="Z57" s="13"/>
+      <c r="AA57" s="13"/>
+      <c r="AB57" s="13"/>
+      <c r="AC57" s="13"/>
+      <c r="AD57" s="13"/>
+      <c r="AE57" s="13"/>
+      <c r="AF57" s="13"/>
+      <c r="AG57" s="13"/>
+      <c r="AH57" s="13"/>
+    </row>
+    <row r="58" spans="1:34">
+      <c r="A58" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B58" s="14">
+      <c r="B58" s="12">
         <v>2</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C58" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="14" t="s">
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="13"/>
+      <c r="U58" s="13"/>
+      <c r="V58" s="13"/>
+      <c r="W58" s="13"/>
+      <c r="X58" s="13"/>
+      <c r="Y58" s="13"/>
+      <c r="Z58" s="13"/>
+      <c r="AA58" s="13"/>
+      <c r="AB58" s="13"/>
+      <c r="AC58" s="13"/>
+      <c r="AD58" s="13"/>
+      <c r="AE58" s="13"/>
+      <c r="AF58" s="13"/>
+      <c r="AG58" s="13"/>
+      <c r="AH58" s="13"/>
+    </row>
+    <row r="59" spans="1:34">
+      <c r="A59" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B59" s="14">
+      <c r="B59" s="12">
         <v>2</v>
       </c>
-      <c r="C59" s="14">
+      <c r="C59" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="14" t="s">
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="13"/>
+      <c r="T59" s="13"/>
+      <c r="U59" s="13"/>
+      <c r="V59" s="13"/>
+      <c r="W59" s="13"/>
+      <c r="X59" s="13"/>
+      <c r="Y59" s="13"/>
+      <c r="Z59" s="13"/>
+      <c r="AA59" s="13"/>
+      <c r="AB59" s="13"/>
+      <c r="AC59" s="13"/>
+      <c r="AD59" s="13"/>
+      <c r="AE59" s="13"/>
+      <c r="AF59" s="13"/>
+      <c r="AG59" s="13"/>
+      <c r="AH59" s="13"/>
+    </row>
+    <row r="60" spans="1:34">
+      <c r="A60" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="B60" s="13">
+      <c r="B60" s="12">
         <v>2</v>
       </c>
-      <c r="C60" s="14">
+      <c r="C60" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="14" t="s">
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+      <c r="S60" s="13"/>
+      <c r="T60" s="13"/>
+      <c r="U60" s="13"/>
+      <c r="V60" s="13"/>
+      <c r="W60" s="13"/>
+      <c r="X60" s="13"/>
+      <c r="Y60" s="13"/>
+      <c r="Z60" s="13"/>
+      <c r="AA60" s="13"/>
+      <c r="AB60" s="13"/>
+      <c r="AC60" s="13"/>
+      <c r="AD60" s="13"/>
+      <c r="AE60" s="13"/>
+      <c r="AF60" s="13"/>
+      <c r="AG60" s="13"/>
+      <c r="AH60" s="13"/>
+    </row>
+    <row r="61" spans="1:34">
+      <c r="A61" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="B61" s="13">
+      <c r="B61" s="12">
         <v>2</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="14" t="s">
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="13"/>
+      <c r="U61" s="13"/>
+      <c r="V61" s="13"/>
+      <c r="W61" s="13"/>
+      <c r="X61" s="13"/>
+      <c r="Y61" s="13"/>
+      <c r="Z61" s="13"/>
+      <c r="AA61" s="13"/>
+      <c r="AB61" s="13"/>
+      <c r="AC61" s="13"/>
+      <c r="AD61" s="13"/>
+      <c r="AE61" s="13"/>
+      <c r="AF61" s="13"/>
+      <c r="AG61" s="13"/>
+      <c r="AH61" s="13"/>
+    </row>
+    <row r="62" spans="1:34">
+      <c r="A62" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B62" s="13">
+      <c r="B62" s="12">
         <v>2</v>
       </c>
-      <c r="C62" s="14">
+      <c r="C62" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="14" t="s">
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13"/>
+      <c r="M62" s="13"/>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13"/>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+      <c r="S62" s="13"/>
+      <c r="T62" s="13"/>
+      <c r="U62" s="13"/>
+      <c r="V62" s="13"/>
+      <c r="W62" s="13"/>
+      <c r="X62" s="13"/>
+      <c r="Y62" s="13"/>
+      <c r="Z62" s="13"/>
+      <c r="AA62" s="13"/>
+      <c r="AB62" s="13"/>
+      <c r="AC62" s="13"/>
+      <c r="AD62" s="13"/>
+      <c r="AE62" s="13"/>
+      <c r="AF62" s="13"/>
+      <c r="AG62" s="13"/>
+      <c r="AH62" s="13"/>
+    </row>
+    <row r="63" spans="1:34">
+      <c r="A63" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B63" s="13">
+      <c r="B63" s="12">
         <v>2</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="14" t="s">
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
+      <c r="S63" s="13"/>
+      <c r="T63" s="13"/>
+      <c r="U63" s="13"/>
+      <c r="V63" s="13"/>
+      <c r="W63" s="13"/>
+      <c r="X63" s="13"/>
+      <c r="Y63" s="13"/>
+      <c r="Z63" s="13"/>
+      <c r="AA63" s="13"/>
+      <c r="AB63" s="13"/>
+      <c r="AC63" s="13"/>
+      <c r="AD63" s="13"/>
+      <c r="AE63" s="13"/>
+      <c r="AF63" s="13"/>
+      <c r="AG63" s="13"/>
+      <c r="AH63" s="13"/>
+    </row>
+    <row r="64" spans="1:34">
+      <c r="A64" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B64" s="13">
+      <c r="B64" s="12">
         <v>2</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C64" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="14" t="s">
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+      <c r="S64" s="13"/>
+      <c r="T64" s="13"/>
+      <c r="U64" s="13"/>
+      <c r="V64" s="13"/>
+      <c r="W64" s="13"/>
+      <c r="X64" s="13"/>
+      <c r="Y64" s="13"/>
+      <c r="Z64" s="13"/>
+      <c r="AA64" s="13"/>
+      <c r="AB64" s="13"/>
+      <c r="AC64" s="13"/>
+      <c r="AD64" s="13"/>
+      <c r="AE64" s="13"/>
+      <c r="AF64" s="13"/>
+      <c r="AG64" s="13"/>
+      <c r="AH64" s="13"/>
+    </row>
+    <row r="65" spans="1:34">
+      <c r="A65" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="B65" s="13">
+      <c r="B65" s="12">
         <v>2</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C65" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="14" t="s">
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="13"/>
+      <c r="U65" s="13"/>
+      <c r="V65" s="13"/>
+      <c r="W65" s="13"/>
+      <c r="X65" s="13"/>
+      <c r="Y65" s="13"/>
+      <c r="Z65" s="13"/>
+      <c r="AA65" s="13"/>
+      <c r="AB65" s="13"/>
+      <c r="AC65" s="13"/>
+      <c r="AD65" s="13"/>
+      <c r="AE65" s="13"/>
+      <c r="AF65" s="13"/>
+      <c r="AG65" s="13"/>
+      <c r="AH65" s="13"/>
+    </row>
+    <row r="66" spans="1:34">
+      <c r="A66" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="B66" s="13">
+      <c r="B66" s="12">
         <v>1</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="14" t="s">
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="13"/>
+      <c r="U66" s="13"/>
+      <c r="V66" s="13"/>
+      <c r="W66" s="13"/>
+      <c r="X66" s="13"/>
+      <c r="Y66" s="13"/>
+      <c r="Z66" s="13"/>
+      <c r="AA66" s="13"/>
+      <c r="AB66" s="13"/>
+      <c r="AC66" s="13"/>
+      <c r="AD66" s="13"/>
+      <c r="AE66" s="13"/>
+      <c r="AF66" s="13"/>
+      <c r="AG66" s="13"/>
+      <c r="AH66" s="13"/>
+    </row>
+    <row r="67" spans="1:34">
+      <c r="A67" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="13">
+      <c r="B67" s="12">
         <v>1</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="14" t="s">
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="13"/>
+      <c r="U67" s="13"/>
+      <c r="V67" s="13"/>
+      <c r="W67" s="13"/>
+      <c r="X67" s="13"/>
+      <c r="Y67" s="13"/>
+      <c r="Z67" s="13"/>
+      <c r="AA67" s="13"/>
+      <c r="AB67" s="13"/>
+      <c r="AC67" s="13"/>
+      <c r="AD67" s="13"/>
+      <c r="AE67" s="13"/>
+      <c r="AF67" s="13"/>
+      <c r="AG67" s="13"/>
+      <c r="AH67" s="13"/>
+    </row>
+    <row r="68" spans="1:34">
+      <c r="A68" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="B68" s="13">
+      <c r="B68" s="12">
         <v>1</v>
       </c>
-      <c r="C68" s="14">
+      <c r="C68" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="14" t="s">
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="13"/>
+      <c r="U68" s="13"/>
+      <c r="V68" s="13"/>
+      <c r="W68" s="13"/>
+      <c r="X68" s="13"/>
+      <c r="Y68" s="13"/>
+      <c r="Z68" s="13"/>
+      <c r="AA68" s="13"/>
+      <c r="AB68" s="13"/>
+      <c r="AC68" s="13"/>
+      <c r="AD68" s="13"/>
+      <c r="AE68" s="13"/>
+      <c r="AF68" s="13"/>
+      <c r="AG68" s="13"/>
+      <c r="AH68" s="13"/>
+    </row>
+    <row r="69" spans="1:34">
+      <c r="A69" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B69" s="13">
+      <c r="B69" s="12">
         <v>1</v>
       </c>
-      <c r="C69" s="14">
+      <c r="C69" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="14" t="s">
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="13"/>
+      <c r="U69" s="13"/>
+      <c r="V69" s="13"/>
+      <c r="W69" s="13"/>
+      <c r="X69" s="13"/>
+      <c r="Y69" s="13"/>
+      <c r="Z69" s="13"/>
+      <c r="AA69" s="13"/>
+      <c r="AB69" s="13"/>
+      <c r="AC69" s="13"/>
+      <c r="AD69" s="13"/>
+      <c r="AE69" s="13"/>
+      <c r="AF69" s="13"/>
+      <c r="AG69" s="13"/>
+      <c r="AH69" s="13"/>
+    </row>
+    <row r="70" spans="1:34">
+      <c r="A70" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B70" s="13">
+      <c r="B70" s="12">
         <v>1</v>
       </c>
-      <c r="C70" s="14">
+      <c r="C70" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="14" t="s">
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="13"/>
+      <c r="U70" s="13"/>
+      <c r="V70" s="13"/>
+      <c r="W70" s="13"/>
+      <c r="X70" s="13"/>
+      <c r="Y70" s="13"/>
+      <c r="Z70" s="13"/>
+      <c r="AA70" s="13"/>
+      <c r="AB70" s="13"/>
+      <c r="AC70" s="13"/>
+      <c r="AD70" s="13"/>
+      <c r="AE70" s="13"/>
+      <c r="AF70" s="13"/>
+      <c r="AG70" s="13"/>
+      <c r="AH70" s="13"/>
+    </row>
+    <row r="71" spans="1:34">
+      <c r="A71" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B71" s="13">
+      <c r="B71" s="12">
         <v>1</v>
       </c>
-      <c r="C71" s="14">
+      <c r="C71" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="14" t="s">
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="13"/>
+      <c r="U71" s="13"/>
+      <c r="V71" s="13"/>
+      <c r="W71" s="13"/>
+      <c r="X71" s="13"/>
+      <c r="Y71" s="13"/>
+      <c r="Z71" s="13"/>
+      <c r="AA71" s="13"/>
+      <c r="AB71" s="13"/>
+      <c r="AC71" s="13"/>
+      <c r="AD71" s="13"/>
+      <c r="AE71" s="13"/>
+      <c r="AF71" s="13"/>
+      <c r="AG71" s="13"/>
+      <c r="AH71" s="13"/>
+    </row>
+    <row r="72" spans="1:34">
+      <c r="A72" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B72" s="13">
+      <c r="B72" s="12">
         <v>1</v>
       </c>
-      <c r="C72" s="14">
+      <c r="C72" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="14" t="s">
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="13"/>
+      <c r="N72" s="13"/>
+      <c r="O72" s="13"/>
+      <c r="P72" s="13"/>
+      <c r="Q72" s="13"/>
+      <c r="R72" s="13"/>
+      <c r="S72" s="13"/>
+      <c r="T72" s="13"/>
+      <c r="U72" s="13"/>
+      <c r="V72" s="13"/>
+      <c r="W72" s="13"/>
+      <c r="X72" s="13"/>
+      <c r="Y72" s="13"/>
+      <c r="Z72" s="13"/>
+      <c r="AA72" s="13"/>
+      <c r="AB72" s="13"/>
+      <c r="AC72" s="13"/>
+      <c r="AD72" s="13"/>
+      <c r="AE72" s="13"/>
+      <c r="AF72" s="13"/>
+      <c r="AG72" s="13"/>
+      <c r="AH72" s="13"/>
+    </row>
+    <row r="73" spans="1:34">
+      <c r="A73" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B73" s="13">
+      <c r="B73" s="12">
         <v>1</v>
       </c>
-      <c r="C73" s="14">
+      <c r="C73" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="14" t="s">
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="13"/>
+      <c r="R73" s="13"/>
+      <c r="S73" s="13"/>
+      <c r="T73" s="13"/>
+      <c r="U73" s="13"/>
+      <c r="V73" s="13"/>
+      <c r="W73" s="13"/>
+      <c r="X73" s="13"/>
+      <c r="Y73" s="13"/>
+      <c r="Z73" s="13"/>
+      <c r="AA73" s="13"/>
+      <c r="AB73" s="13"/>
+      <c r="AC73" s="13"/>
+      <c r="AD73" s="13"/>
+      <c r="AE73" s="13"/>
+      <c r="AF73" s="13"/>
+      <c r="AG73" s="13"/>
+      <c r="AH73" s="13"/>
+    </row>
+    <row r="74" spans="1:34">
+      <c r="A74" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B74" s="13">
+      <c r="B74" s="12">
         <v>1</v>
       </c>
-      <c r="C74" s="14">
+      <c r="C74" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="14" t="s">
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13"/>
+      <c r="O74" s="13"/>
+      <c r="P74" s="13"/>
+      <c r="Q74" s="13"/>
+      <c r="R74" s="13"/>
+      <c r="S74" s="13"/>
+      <c r="T74" s="13"/>
+      <c r="U74" s="13"/>
+      <c r="V74" s="13"/>
+      <c r="W74" s="13"/>
+      <c r="X74" s="13"/>
+      <c r="Y74" s="13"/>
+      <c r="Z74" s="13"/>
+      <c r="AA74" s="13"/>
+      <c r="AB74" s="13"/>
+      <c r="AC74" s="13"/>
+      <c r="AD74" s="13"/>
+      <c r="AE74" s="13"/>
+      <c r="AF74" s="13"/>
+      <c r="AG74" s="13"/>
+      <c r="AH74" s="13"/>
+    </row>
+    <row r="75" spans="1:34">
+      <c r="A75" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B75" s="13">
+      <c r="B75" s="12">
         <v>1</v>
       </c>
-      <c r="C75" s="14">
+      <c r="C75" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="13"/>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="13"/>
+      <c r="R75" s="13"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="13"/>
+      <c r="U75" s="13"/>
+      <c r="V75" s="13"/>
+      <c r="W75" s="13"/>
+      <c r="X75" s="13"/>
+      <c r="Y75" s="13"/>
+      <c r="Z75" s="13"/>
+      <c r="AA75" s="13"/>
+      <c r="AB75" s="13"/>
+      <c r="AC75" s="13"/>
+      <c r="AD75" s="13"/>
+      <c r="AE75" s="13"/>
+      <c r="AF75" s="13"/>
+      <c r="AG75" s="13"/>
+      <c r="AH75" s="13"/>
+    </row>
+    <row r="76" spans="1:34">
       <c r="A76" s="11"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:34">
       <c r="A77" s="11"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:34">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:34">
       <c r="A79" s="11"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:34">
       <c r="A80" s="11"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -3666,7 +6085,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>